<commit_message>
CES-3359 Add write capability to volume key for snapshot support
</commit_message>
<xml_diff>
--- a/osp_deployer/settings/CWD_Mercury/mercury.xlsx
+++ b/osp_deployer/settings/CWD_Mercury/mercury.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\deploy-auto\osp_deployer\settings\mercury\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\deploy-auto\osp_deployer\settings\CWD_Mercury\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="11736" windowHeight="4236" tabRatio="782" firstSheet="4" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="11736" windowHeight="4236" tabRatio="782" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" state="hidden" r:id="rId1"/>
@@ -2461,13 +2461,13 @@
     <t>EQL Arrays</t>
   </si>
   <si>
-    <t>120, 140, 170, 190</t>
-  </si>
-  <si>
     <t xml:space="preserve">SAH Puiblic Install NIC --- </t>
   </si>
   <si>
     <t>3990</t>
+  </si>
+  <si>
+    <t>110,120, 140, 170, 190</t>
   </si>
 </sst>
 </file>
@@ -7443,6 +7443,45 @@
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="39" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="40" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="41" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="37" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="6" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="38" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="28" borderId="19" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="20" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="21" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="34" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="35" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="26" borderId="35" xfId="141" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="36" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="37" fillId="26" borderId="19" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -7482,60 +7521,145 @@
     <xf numFmtId="0" fontId="43" fillId="27" borderId="33" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="28" borderId="19" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="20" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="21" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="34" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="35" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="26" borderId="35" xfId="141" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="36" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="39" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="40" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="41" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="37" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="6" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="38" xfId="141" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="44" fillId="27" borderId="58" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="27" borderId="12" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="27" borderId="59" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="41" borderId="58" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="41" borderId="12" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="41" borderId="59" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="27" borderId="31" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="27" borderId="32" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="27" borderId="33" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="19" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="20" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="21" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="22" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="23" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="24" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="8" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="25" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="81" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="81" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="81" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="27" borderId="82" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="27" borderId="77" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="27" borderId="83" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="58" xfId="112" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="12" xfId="112" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="59" xfId="112" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="41" borderId="39" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="60" fillId="41" borderId="40" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="53" fillId="41" borderId="40" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -7549,10 +7673,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="58" xfId="1629" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="58" xfId="112" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -7570,126 +7690,6 @@
     <xf numFmtId="0" fontId="60" fillId="41" borderId="37" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="60" fillId="41" borderId="6" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="53" fillId="41" borderId="6" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="41" borderId="58" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="41" borderId="12" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="41" borderId="59" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="12" xfId="112" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="59" xfId="112" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="27" borderId="82" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="27" borderId="12" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="27" borderId="59" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="27" borderId="77" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="27" borderId="83" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="27" borderId="58" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="27" borderId="31" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="27" borderId="32" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="27" borderId="33" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="19" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="20" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="21" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="22" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="23" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="24" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="8" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="25" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="81" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="81" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="81" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="1628" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="1628" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="48" fillId="25" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7718,6 +7718,35 @@
     </xf>
     <xf numFmtId="0" fontId="49" fillId="25" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="37" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="36" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="31" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="31" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="33" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="31" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="36" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="36" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="36" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="38" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="32" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="32" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
@@ -7725,35 +7754,6 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="57" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="46" fillId="31" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="31" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="36" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="36" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="36" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="33" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="38" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="32" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="36" fillId="32" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="37" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="36" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="46" fillId="31" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="100" fillId="0" borderId="96" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -11506,19 +11506,19 @@
     </row>
     <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
-      <c r="B7" s="284" t="s">
+      <c r="B7" s="297" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="285"/>
-      <c r="D7" s="285"/>
-      <c r="E7" s="285"/>
-      <c r="F7" s="285"/>
-      <c r="G7" s="285"/>
-      <c r="H7" s="285"/>
-      <c r="I7" s="285"/>
-      <c r="J7" s="285"/>
-      <c r="K7" s="285"/>
-      <c r="L7" s="286"/>
+      <c r="C7" s="298"/>
+      <c r="D7" s="298"/>
+      <c r="E7" s="298"/>
+      <c r="F7" s="298"/>
+      <c r="G7" s="298"/>
+      <c r="H7" s="298"/>
+      <c r="I7" s="298"/>
+      <c r="J7" s="298"/>
+      <c r="K7" s="298"/>
+      <c r="L7" s="299"/>
       <c r="M7" s="9"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11606,19 +11606,19 @@
     </row>
     <row r="13" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
-      <c r="B13" s="287" t="s">
+      <c r="B13" s="300" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="288"/>
-      <c r="D13" s="288"/>
-      <c r="E13" s="288"/>
-      <c r="F13" s="288"/>
-      <c r="G13" s="288"/>
-      <c r="H13" s="288"/>
-      <c r="I13" s="288"/>
-      <c r="J13" s="288"/>
-      <c r="K13" s="288"/>
-      <c r="L13" s="289"/>
+      <c r="C13" s="301"/>
+      <c r="D13" s="301"/>
+      <c r="E13" s="301"/>
+      <c r="F13" s="301"/>
+      <c r="G13" s="301"/>
+      <c r="H13" s="301"/>
+      <c r="I13" s="301"/>
+      <c r="J13" s="301"/>
+      <c r="K13" s="301"/>
+      <c r="L13" s="302"/>
       <c r="M13" s="9"/>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11706,19 +11706,19 @@
     </row>
     <row r="19" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
-      <c r="B19" s="290" t="s">
+      <c r="B19" s="303" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="291"/>
-      <c r="D19" s="291"/>
-      <c r="E19" s="291"/>
-      <c r="F19" s="291"/>
-      <c r="G19" s="291"/>
-      <c r="H19" s="291"/>
-      <c r="I19" s="291"/>
-      <c r="J19" s="291"/>
-      <c r="K19" s="291"/>
-      <c r="L19" s="292"/>
+      <c r="C19" s="304"/>
+      <c r="D19" s="304"/>
+      <c r="E19" s="304"/>
+      <c r="F19" s="304"/>
+      <c r="G19" s="304"/>
+      <c r="H19" s="304"/>
+      <c r="I19" s="304"/>
+      <c r="J19" s="304"/>
+      <c r="K19" s="304"/>
+      <c r="L19" s="305"/>
       <c r="M19" s="9"/>
     </row>
     <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11789,19 +11789,19 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
-      <c r="B24" s="293" t="s">
+      <c r="B24" s="306" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="294"/>
-      <c r="D24" s="294"/>
-      <c r="E24" s="294"/>
-      <c r="F24" s="294"/>
-      <c r="G24" s="294"/>
-      <c r="H24" s="294"/>
-      <c r="I24" s="294"/>
-      <c r="J24" s="294"/>
-      <c r="K24" s="294"/>
-      <c r="L24" s="295"/>
+      <c r="C24" s="307"/>
+      <c r="D24" s="307"/>
+      <c r="E24" s="307"/>
+      <c r="F24" s="307"/>
+      <c r="G24" s="307"/>
+      <c r="H24" s="307"/>
+      <c r="I24" s="307"/>
+      <c r="J24" s="307"/>
+      <c r="K24" s="307"/>
+      <c r="L24" s="308"/>
       <c r="M24" s="9"/>
     </row>
     <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11957,110 +11957,110 @@
     </row>
     <row r="34" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4"/>
-      <c r="B34" s="296" t="s">
+      <c r="B34" s="309" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="297"/>
-      <c r="D34" s="297"/>
-      <c r="E34" s="297"/>
-      <c r="F34" s="297"/>
-      <c r="G34" s="297"/>
-      <c r="H34" s="297"/>
-      <c r="I34" s="297"/>
-      <c r="J34" s="297"/>
-      <c r="K34" s="297"/>
-      <c r="L34" s="298"/>
+      <c r="C34" s="310"/>
+      <c r="D34" s="310"/>
+      <c r="E34" s="310"/>
+      <c r="F34" s="310"/>
+      <c r="G34" s="310"/>
+      <c r="H34" s="310"/>
+      <c r="I34" s="310"/>
+      <c r="J34" s="310"/>
+      <c r="K34" s="310"/>
+      <c r="L34" s="311"/>
       <c r="M34" s="9"/>
     </row>
     <row r="35" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4"/>
-      <c r="B35" s="299" t="s">
+      <c r="B35" s="290" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="300"/>
-      <c r="D35" s="301"/>
-      <c r="E35" s="299" t="s">
+      <c r="C35" s="291"/>
+      <c r="D35" s="292"/>
+      <c r="E35" s="290" t="s">
         <v>26</v>
       </c>
-      <c r="F35" s="300"/>
-      <c r="G35" s="301"/>
-      <c r="H35" s="299" t="s">
+      <c r="F35" s="291"/>
+      <c r="G35" s="292"/>
+      <c r="H35" s="290" t="s">
         <v>27</v>
       </c>
-      <c r="I35" s="300"/>
-      <c r="J35" s="301"/>
-      <c r="K35" s="299" t="s">
+      <c r="I35" s="291"/>
+      <c r="J35" s="292"/>
+      <c r="K35" s="290" t="s">
         <v>28</v>
       </c>
-      <c r="L35" s="301"/>
+      <c r="L35" s="292"/>
       <c r="M35" s="9"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
-      <c r="B36" s="302">
+      <c r="B36" s="293">
         <v>1</v>
       </c>
-      <c r="C36" s="303"/>
-      <c r="D36" s="303"/>
-      <c r="E36" s="304"/>
-      <c r="F36" s="303"/>
-      <c r="G36" s="303"/>
-      <c r="H36" s="303"/>
-      <c r="I36" s="303"/>
-      <c r="J36" s="303"/>
-      <c r="K36" s="303"/>
-      <c r="L36" s="305"/>
+      <c r="C36" s="294"/>
+      <c r="D36" s="294"/>
+      <c r="E36" s="295"/>
+      <c r="F36" s="294"/>
+      <c r="G36" s="294"/>
+      <c r="H36" s="294"/>
+      <c r="I36" s="294"/>
+      <c r="J36" s="294"/>
+      <c r="K36" s="294"/>
+      <c r="L36" s="296"/>
       <c r="M36" s="9"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
-      <c r="B37" s="309">
+      <c r="B37" s="287">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C37" s="310"/>
-      <c r="D37" s="310"/>
-      <c r="E37" s="310"/>
-      <c r="F37" s="310"/>
-      <c r="G37" s="310"/>
-      <c r="H37" s="310"/>
-      <c r="I37" s="310"/>
-      <c r="J37" s="310"/>
-      <c r="K37" s="310"/>
-      <c r="L37" s="311"/>
+      <c r="C37" s="288"/>
+      <c r="D37" s="288"/>
+      <c r="E37" s="288"/>
+      <c r="F37" s="288"/>
+      <c r="G37" s="288"/>
+      <c r="H37" s="288"/>
+      <c r="I37" s="288"/>
+      <c r="J37" s="288"/>
+      <c r="K37" s="288"/>
+      <c r="L37" s="289"/>
       <c r="M37" s="9"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
-      <c r="B38" s="309">
+      <c r="B38" s="287">
         <v>1.2</v>
       </c>
-      <c r="C38" s="310"/>
-      <c r="D38" s="310"/>
-      <c r="E38" s="310"/>
-      <c r="F38" s="310"/>
-      <c r="G38" s="310"/>
-      <c r="H38" s="310"/>
-      <c r="I38" s="310"/>
-      <c r="J38" s="310"/>
-      <c r="K38" s="310"/>
-      <c r="L38" s="311"/>
+      <c r="C38" s="288"/>
+      <c r="D38" s="288"/>
+      <c r="E38" s="288"/>
+      <c r="F38" s="288"/>
+      <c r="G38" s="288"/>
+      <c r="H38" s="288"/>
+      <c r="I38" s="288"/>
+      <c r="J38" s="288"/>
+      <c r="K38" s="288"/>
+      <c r="L38" s="289"/>
       <c r="M38" s="9"/>
     </row>
     <row r="39" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="4"/>
-      <c r="B39" s="306">
+      <c r="B39" s="284">
         <v>1.3</v>
       </c>
-      <c r="C39" s="307"/>
-      <c r="D39" s="307"/>
-      <c r="E39" s="307"/>
-      <c r="F39" s="307"/>
-      <c r="G39" s="307"/>
-      <c r="H39" s="307"/>
-      <c r="I39" s="307"/>
-      <c r="J39" s="307"/>
-      <c r="K39" s="307"/>
-      <c r="L39" s="308"/>
+      <c r="C39" s="285"/>
+      <c r="D39" s="285"/>
+      <c r="E39" s="285"/>
+      <c r="F39" s="285"/>
+      <c r="G39" s="285"/>
+      <c r="H39" s="285"/>
+      <c r="I39" s="285"/>
+      <c r="J39" s="285"/>
+      <c r="K39" s="285"/>
+      <c r="L39" s="286"/>
       <c r="M39" s="9"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
@@ -12080,6 +12080,19 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B7:L7"/>
+    <mergeCell ref="B13:L13"/>
+    <mergeCell ref="B19:L19"/>
+    <mergeCell ref="B24:L24"/>
+    <mergeCell ref="B34:L34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:J35"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="K36:L36"/>
     <mergeCell ref="B39:D39"/>
     <mergeCell ref="E39:G39"/>
     <mergeCell ref="H39:J39"/>
@@ -12092,19 +12105,6 @@
     <mergeCell ref="E38:G38"/>
     <mergeCell ref="H38:J38"/>
     <mergeCell ref="K38:L38"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:J35"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="B7:L7"/>
-    <mergeCell ref="B13:L13"/>
-    <mergeCell ref="B19:L19"/>
-    <mergeCell ref="B24:L24"/>
-    <mergeCell ref="B34:L34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -12155,28 +12155,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="L2" s="391" t="s">
+      <c r="L2" s="375" t="s">
         <v>79</v>
       </c>
-      <c r="M2" s="391"/>
-      <c r="N2" s="391"/>
-      <c r="O2" s="391"/>
-      <c r="P2" s="391"/>
-      <c r="Q2" s="391"/>
-      <c r="R2" s="391"/>
-      <c r="S2" s="391"/>
+      <c r="M2" s="375"/>
+      <c r="N2" s="375"/>
+      <c r="O2" s="375"/>
+      <c r="P2" s="375"/>
+      <c r="Q2" s="375"/>
+      <c r="R2" s="375"/>
+      <c r="S2" s="375"/>
     </row>
     <row r="3" spans="2:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="392" t="s">
+      <c r="B3" s="376" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="392"/>
-      <c r="D3" s="388" t="s">
+      <c r="C3" s="376"/>
+      <c r="D3" s="377" t="s">
         <v>321</v>
       </c>
-      <c r="E3" s="388"/>
-      <c r="F3" s="388"/>
-      <c r="G3" s="388"/>
+      <c r="E3" s="377"/>
+      <c r="F3" s="377"/>
+      <c r="G3" s="377"/>
       <c r="I3" s="368" t="s">
         <v>49</v>
       </c>
@@ -12184,31 +12184,31 @@
       <c r="L3" s="381" t="s">
         <v>37</v>
       </c>
-      <c r="M3" s="393"/>
-      <c r="N3" s="393" t="s">
+      <c r="M3" s="378"/>
+      <c r="N3" s="378" t="s">
         <v>54</v>
       </c>
-      <c r="O3" s="393"/>
-      <c r="P3" s="393" t="s">
+      <c r="O3" s="378"/>
+      <c r="P3" s="378" t="s">
         <v>49</v>
       </c>
-      <c r="Q3" s="393"/>
-      <c r="R3" s="393" t="s">
+      <c r="Q3" s="378"/>
+      <c r="R3" s="378" t="s">
         <v>50</v>
       </c>
-      <c r="S3" s="382"/>
+      <c r="S3" s="379"/>
     </row>
     <row r="4" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="B4" s="386" t="s">
+      <c r="B4" s="380" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="386"/>
-      <c r="D4" s="388" t="s">
+      <c r="C4" s="380"/>
+      <c r="D4" s="377" t="s">
         <v>322</v>
       </c>
-      <c r="E4" s="388"/>
-      <c r="F4" s="388"/>
-      <c r="G4" s="388"/>
+      <c r="E4" s="377"/>
+      <c r="F4" s="377"/>
+      <c r="G4" s="377"/>
       <c r="I4" s="39" t="s">
         <v>80</v>
       </c>
@@ -12265,16 +12265,16 @@
       </c>
     </row>
     <row r="5" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="B5" s="392" t="s">
+      <c r="B5" s="376" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="392"/>
-      <c r="D5" s="388" t="s">
+      <c r="C5" s="376"/>
+      <c r="D5" s="377" t="s">
         <v>323</v>
       </c>
-      <c r="E5" s="388"/>
-      <c r="F5" s="388"/>
-      <c r="G5" s="388"/>
+      <c r="E5" s="377"/>
+      <c r="F5" s="377"/>
+      <c r="G5" s="377"/>
       <c r="I5" s="39" t="s">
         <v>307</v>
       </c>
@@ -12321,14 +12321,14 @@
       </c>
     </row>
     <row r="6" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="B6" s="386" t="s">
+      <c r="B6" s="380" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="386"/>
-      <c r="D6" s="388"/>
-      <c r="E6" s="388"/>
-      <c r="F6" s="388"/>
-      <c r="G6" s="388"/>
+      <c r="C6" s="380"/>
+      <c r="D6" s="377"/>
+      <c r="E6" s="377"/>
+      <c r="F6" s="377"/>
+      <c r="G6" s="377"/>
       <c r="I6" s="39">
         <v>121</v>
       </c>
@@ -12414,16 +12414,16 @@
       </c>
     </row>
     <row r="8" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="B8" s="390" t="s">
+      <c r="B8" s="387" t="s">
         <v>233</v>
       </c>
-      <c r="C8" s="390"/>
-      <c r="D8" s="390"/>
-      <c r="E8" s="388" t="s">
+      <c r="C8" s="387"/>
+      <c r="D8" s="387"/>
+      <c r="E8" s="377" t="s">
         <v>235</v>
       </c>
-      <c r="F8" s="388"/>
-      <c r="G8" s="388"/>
+      <c r="F8" s="377"/>
+      <c r="G8" s="377"/>
       <c r="I8" s="39"/>
       <c r="J8" s="39"/>
       <c r="L8" s="35" t="s">
@@ -12460,16 +12460,16 @@
       </c>
     </row>
     <row r="9" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="B9" s="387" t="s">
+      <c r="B9" s="385" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="387"/>
-      <c r="D9" s="387"/>
-      <c r="E9" s="388" t="s">
+      <c r="C9" s="385"/>
+      <c r="D9" s="385"/>
+      <c r="E9" s="377" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="388"/>
-      <c r="G9" s="388"/>
+      <c r="F9" s="377"/>
+      <c r="G9" s="377"/>
       <c r="I9" s="39"/>
       <c r="J9" s="39"/>
       <c r="L9" s="35" t="s">
@@ -12506,16 +12506,16 @@
       </c>
     </row>
     <row r="10" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="B10" s="389" t="s">
+      <c r="B10" s="386" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="389"/>
-      <c r="D10" s="389"/>
-      <c r="E10" s="388">
+      <c r="C10" s="386"/>
+      <c r="D10" s="386"/>
+      <c r="E10" s="377">
         <v>12288</v>
       </c>
-      <c r="F10" s="388"/>
-      <c r="G10" s="388"/>
+      <c r="F10" s="377"/>
+      <c r="G10" s="377"/>
       <c r="I10" s="39"/>
       <c r="J10" s="39"/>
       <c r="L10" s="35" t="s">
@@ -12580,20 +12580,20 @@
       </c>
     </row>
     <row r="12" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="B12" s="390" t="s">
+      <c r="B12" s="387" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="390"/>
-      <c r="D12" s="390"/>
-      <c r="E12" s="388" t="s">
+      <c r="C12" s="387"/>
+      <c r="D12" s="387"/>
+      <c r="E12" s="377" t="s">
         <v>65</v>
       </c>
-      <c r="F12" s="388"/>
-      <c r="G12" s="388"/>
+      <c r="F12" s="377"/>
+      <c r="G12" s="377"/>
       <c r="I12" s="381" t="s">
         <v>75</v>
       </c>
-      <c r="J12" s="382"/>
+      <c r="J12" s="379"/>
       <c r="L12" s="35" t="s">
         <v>156</v>
       </c>
@@ -12662,14 +12662,14 @@
       </c>
     </row>
     <row r="14" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="B14" s="383" t="s">
+      <c r="B14" s="382" t="s">
         <v>81</v>
       </c>
-      <c r="C14" s="384"/>
-      <c r="D14" s="384"/>
-      <c r="E14" s="384"/>
-      <c r="F14" s="384"/>
-      <c r="G14" s="385"/>
+      <c r="C14" s="383"/>
+      <c r="D14" s="383"/>
+      <c r="E14" s="383"/>
+      <c r="F14" s="383"/>
+      <c r="G14" s="384"/>
       <c r="I14" s="39" t="s">
         <v>48</v>
       </c>
@@ -12705,12 +12705,12 @@
       </c>
     </row>
     <row r="15" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="B15" s="375"/>
-      <c r="C15" s="376"/>
-      <c r="D15" s="376"/>
-      <c r="E15" s="376"/>
-      <c r="F15" s="376"/>
-      <c r="G15" s="377"/>
+      <c r="B15" s="388"/>
+      <c r="C15" s="389"/>
+      <c r="D15" s="389"/>
+      <c r="E15" s="389"/>
+      <c r="F15" s="389"/>
+      <c r="G15" s="390"/>
       <c r="I15" s="39" t="s">
         <v>73</v>
       </c>
@@ -12746,12 +12746,12 @@
       </c>
     </row>
     <row r="16" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="B16" s="378"/>
-      <c r="C16" s="379"/>
-      <c r="D16" s="379"/>
-      <c r="E16" s="379"/>
-      <c r="F16" s="379"/>
-      <c r="G16" s="380"/>
+      <c r="B16" s="391"/>
+      <c r="C16" s="392"/>
+      <c r="D16" s="392"/>
+      <c r="E16" s="392"/>
+      <c r="F16" s="392"/>
+      <c r="G16" s="393"/>
       <c r="I16" s="39" t="s">
         <v>74</v>
       </c>
@@ -12787,12 +12787,12 @@
       </c>
     </row>
     <row r="17" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="B17" s="375"/>
-      <c r="C17" s="376"/>
-      <c r="D17" s="376"/>
-      <c r="E17" s="376"/>
-      <c r="F17" s="376"/>
-      <c r="G17" s="377"/>
+      <c r="B17" s="388"/>
+      <c r="C17" s="389"/>
+      <c r="D17" s="389"/>
+      <c r="E17" s="389"/>
+      <c r="F17" s="389"/>
+      <c r="G17" s="390"/>
       <c r="I17" s="39"/>
       <c r="J17" s="39"/>
       <c r="L17" s="35" t="s">
@@ -12823,12 +12823,12 @@
       </c>
     </row>
     <row r="18" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="B18" s="378"/>
-      <c r="C18" s="379"/>
-      <c r="D18" s="379"/>
-      <c r="E18" s="379"/>
-      <c r="F18" s="379"/>
-      <c r="G18" s="380"/>
+      <c r="B18" s="391"/>
+      <c r="C18" s="392"/>
+      <c r="D18" s="392"/>
+      <c r="E18" s="392"/>
+      <c r="F18" s="392"/>
+      <c r="G18" s="393"/>
       <c r="I18" s="39"/>
       <c r="J18" s="39"/>
       <c r="L18" s="35" t="s">
@@ -14021,6 +14021,23 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:G8"/>
     <mergeCell ref="L2:S2"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:G5"/>
@@ -14033,23 +14050,6 @@
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="N3:O3"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="I22:J22"/>
   </mergeCells>
   <dataValidations count="8">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9:G9">
@@ -14723,7 +14723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
@@ -15512,15 +15512,15 @@
     </row>
     <row r="2" spans="1:14" s="78" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="77"/>
-      <c r="B2" s="345" t="s">
+      <c r="B2" s="312" t="s">
         <v>206</v>
       </c>
-      <c r="C2" s="341"/>
-      <c r="D2" s="341"/>
-      <c r="E2" s="341"/>
-      <c r="F2" s="341"/>
-      <c r="G2" s="341"/>
-      <c r="H2" s="342"/>
+      <c r="C2" s="313"/>
+      <c r="D2" s="313"/>
+      <c r="E2" s="313"/>
+      <c r="F2" s="313"/>
+      <c r="G2" s="313"/>
+      <c r="H2" s="314"/>
       <c r="I2" s="77"/>
       <c r="J2" s="77"/>
       <c r="K2" s="77"/>
@@ -15530,124 +15530,124 @@
     </row>
     <row r="3" spans="1:14" s="78" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="77"/>
-      <c r="B3" s="334" t="s">
+      <c r="B3" s="315" t="s">
         <v>207</v>
       </c>
-      <c r="C3" s="335"/>
-      <c r="D3" s="336"/>
-      <c r="E3" s="334" t="s">
+      <c r="C3" s="316"/>
+      <c r="D3" s="317"/>
+      <c r="E3" s="315" t="s">
         <v>208</v>
       </c>
-      <c r="F3" s="335"/>
-      <c r="G3" s="335"/>
-      <c r="H3" s="336"/>
+      <c r="F3" s="316"/>
+      <c r="G3" s="316"/>
+      <c r="H3" s="317"/>
       <c r="I3" s="77"/>
       <c r="J3" s="77"/>
-      <c r="K3" s="346" t="s">
+      <c r="K3" s="318" t="s">
         <v>209</v>
       </c>
-      <c r="L3" s="347"/>
-      <c r="M3" s="348"/>
+      <c r="L3" s="319"/>
+      <c r="M3" s="320"/>
       <c r="N3" s="77"/>
     </row>
     <row r="4" spans="1:14" s="78" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="77"/>
-      <c r="B4" s="331"/>
-      <c r="C4" s="332"/>
-      <c r="D4" s="333"/>
-      <c r="E4" s="315"/>
-      <c r="F4" s="316"/>
-      <c r="G4" s="316"/>
-      <c r="H4" s="317"/>
+      <c r="B4" s="321"/>
+      <c r="C4" s="322"/>
+      <c r="D4" s="323"/>
+      <c r="E4" s="324"/>
+      <c r="F4" s="325"/>
+      <c r="G4" s="325"/>
+      <c r="H4" s="326"/>
       <c r="I4" s="77"/>
       <c r="J4" s="77"/>
-      <c r="K4" s="349"/>
-      <c r="L4" s="350"/>
-      <c r="M4" s="351"/>
+      <c r="K4" s="327"/>
+      <c r="L4" s="328"/>
+      <c r="M4" s="329"/>
       <c r="N4" s="77"/>
     </row>
     <row r="5" spans="1:14" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="77"/>
-      <c r="B5" s="334" t="s">
+      <c r="B5" s="315" t="s">
         <v>287</v>
       </c>
-      <c r="C5" s="335"/>
-      <c r="D5" s="335"/>
-      <c r="E5" s="334" t="s">
+      <c r="C5" s="316"/>
+      <c r="D5" s="316"/>
+      <c r="E5" s="315" t="s">
         <v>210</v>
       </c>
-      <c r="F5" s="335"/>
-      <c r="G5" s="335"/>
-      <c r="H5" s="336"/>
+      <c r="F5" s="316"/>
+      <c r="G5" s="316"/>
+      <c r="H5" s="317"/>
       <c r="I5" s="77"/>
       <c r="J5" s="79"/>
-      <c r="K5" s="352"/>
-      <c r="L5" s="353"/>
-      <c r="M5" s="354"/>
+      <c r="K5" s="330"/>
+      <c r="L5" s="331"/>
+      <c r="M5" s="332"/>
       <c r="N5" s="77"/>
     </row>
     <row r="6" spans="1:14" s="78" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="77"/>
-      <c r="B6" s="358"/>
-      <c r="C6" s="359"/>
-      <c r="D6" s="359"/>
-      <c r="E6" s="360"/>
-      <c r="F6" s="360"/>
-      <c r="G6" s="360"/>
-      <c r="H6" s="360"/>
+      <c r="B6" s="336"/>
+      <c r="C6" s="337"/>
+      <c r="D6" s="337"/>
+      <c r="E6" s="338"/>
+      <c r="F6" s="338"/>
+      <c r="G6" s="338"/>
+      <c r="H6" s="338"/>
       <c r="I6" s="77"/>
       <c r="J6" s="79"/>
-      <c r="K6" s="352"/>
-      <c r="L6" s="353"/>
-      <c r="M6" s="354"/>
+      <c r="K6" s="330"/>
+      <c r="L6" s="331"/>
+      <c r="M6" s="332"/>
       <c r="N6" s="77"/>
     </row>
     <row r="7" spans="1:14" s="78" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="77"/>
-      <c r="B7" s="361"/>
-      <c r="C7" s="361"/>
-      <c r="D7" s="361"/>
-      <c r="E7" s="362"/>
-      <c r="F7" s="362"/>
-      <c r="G7" s="362"/>
-      <c r="H7" s="362"/>
+      <c r="B7" s="339"/>
+      <c r="C7" s="339"/>
+      <c r="D7" s="339"/>
+      <c r="E7" s="340"/>
+      <c r="F7" s="340"/>
+      <c r="G7" s="340"/>
+      <c r="H7" s="340"/>
       <c r="I7" s="77"/>
       <c r="J7" s="77"/>
-      <c r="K7" s="352"/>
-      <c r="L7" s="353"/>
-      <c r="M7" s="354"/>
+      <c r="K7" s="330"/>
+      <c r="L7" s="331"/>
+      <c r="M7" s="332"/>
       <c r="N7" s="77"/>
     </row>
     <row r="8" spans="1:14" s="78" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="77"/>
-      <c r="B8" s="361"/>
-      <c r="C8" s="361"/>
-      <c r="D8" s="361"/>
-      <c r="E8" s="362"/>
-      <c r="F8" s="362"/>
-      <c r="G8" s="362"/>
-      <c r="H8" s="362"/>
+      <c r="B8" s="339"/>
+      <c r="C8" s="339"/>
+      <c r="D8" s="339"/>
+      <c r="E8" s="340"/>
+      <c r="F8" s="340"/>
+      <c r="G8" s="340"/>
+      <c r="H8" s="340"/>
       <c r="I8" s="77"/>
       <c r="J8" s="77"/>
-      <c r="K8" s="352"/>
-      <c r="L8" s="353"/>
-      <c r="M8" s="354"/>
+      <c r="K8" s="330"/>
+      <c r="L8" s="331"/>
+      <c r="M8" s="332"/>
       <c r="N8" s="77"/>
     </row>
     <row r="9" spans="1:14" s="78" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="77"/>
-      <c r="B9" s="363"/>
-      <c r="C9" s="363"/>
-      <c r="D9" s="363"/>
-      <c r="E9" s="339"/>
-      <c r="F9" s="339"/>
-      <c r="G9" s="339"/>
-      <c r="H9" s="339"/>
+      <c r="B9" s="341"/>
+      <c r="C9" s="341"/>
+      <c r="D9" s="341"/>
+      <c r="E9" s="342"/>
+      <c r="F9" s="342"/>
+      <c r="G9" s="342"/>
+      <c r="H9" s="342"/>
       <c r="I9" s="77"/>
       <c r="J9" s="77"/>
-      <c r="K9" s="352"/>
-      <c r="L9" s="353"/>
-      <c r="M9" s="354"/>
+      <c r="K9" s="330"/>
+      <c r="L9" s="331"/>
+      <c r="M9" s="332"/>
       <c r="N9" s="77"/>
     </row>
     <row r="10" spans="1:14" s="78" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -15661,47 +15661,47 @@
       <c r="H10" s="81"/>
       <c r="I10" s="77"/>
       <c r="J10" s="77"/>
-      <c r="K10" s="352"/>
-      <c r="L10" s="353"/>
-      <c r="M10" s="354"/>
+      <c r="K10" s="330"/>
+      <c r="L10" s="331"/>
+      <c r="M10" s="332"/>
       <c r="N10" s="77"/>
     </row>
     <row r="11" spans="1:14" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="77"/>
-      <c r="B11" s="340" t="s">
+      <c r="B11" s="343" t="s">
         <v>211</v>
       </c>
-      <c r="C11" s="341"/>
-      <c r="D11" s="341"/>
-      <c r="E11" s="341"/>
-      <c r="F11" s="341"/>
-      <c r="G11" s="341"/>
-      <c r="H11" s="342"/>
+      <c r="C11" s="313"/>
+      <c r="D11" s="313"/>
+      <c r="E11" s="313"/>
+      <c r="F11" s="313"/>
+      <c r="G11" s="313"/>
+      <c r="H11" s="314"/>
       <c r="I11" s="77"/>
       <c r="J11" s="77"/>
-      <c r="K11" s="352"/>
-      <c r="L11" s="353"/>
-      <c r="M11" s="354"/>
+      <c r="K11" s="330"/>
+      <c r="L11" s="331"/>
+      <c r="M11" s="332"/>
       <c r="N11" s="77"/>
     </row>
     <row r="12" spans="1:14" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="77"/>
       <c r="B12" s="82"/>
-      <c r="C12" s="334" t="s">
+      <c r="C12" s="315" t="s">
         <v>212</v>
       </c>
-      <c r="D12" s="335"/>
-      <c r="E12" s="335"/>
-      <c r="F12" s="334" t="s">
+      <c r="D12" s="316"/>
+      <c r="E12" s="316"/>
+      <c r="F12" s="315" t="s">
         <v>213</v>
       </c>
-      <c r="G12" s="335"/>
-      <c r="H12" s="336"/>
+      <c r="G12" s="316"/>
+      <c r="H12" s="317"/>
       <c r="I12" s="77"/>
       <c r="J12" s="77"/>
-      <c r="K12" s="352"/>
-      <c r="L12" s="353"/>
-      <c r="M12" s="354"/>
+      <c r="K12" s="330"/>
+      <c r="L12" s="331"/>
+      <c r="M12" s="332"/>
       <c r="N12" s="77"/>
     </row>
     <row r="13" spans="1:14" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -15709,17 +15709,17 @@
       <c r="B13" s="83" t="s">
         <v>71</v>
       </c>
-      <c r="C13" s="315"/>
-      <c r="D13" s="316"/>
-      <c r="E13" s="317"/>
-      <c r="F13" s="331"/>
-      <c r="G13" s="332"/>
-      <c r="H13" s="333"/>
+      <c r="C13" s="324"/>
+      <c r="D13" s="325"/>
+      <c r="E13" s="326"/>
+      <c r="F13" s="321"/>
+      <c r="G13" s="322"/>
+      <c r="H13" s="323"/>
       <c r="I13" s="77"/>
       <c r="J13" s="77"/>
-      <c r="K13" s="352"/>
-      <c r="L13" s="353"/>
-      <c r="M13" s="354"/>
+      <c r="K13" s="330"/>
+      <c r="L13" s="331"/>
+      <c r="M13" s="332"/>
       <c r="N13" s="77"/>
     </row>
     <row r="14" spans="1:14" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -15727,17 +15727,17 @@
       <c r="B14" s="84" t="s">
         <v>214</v>
       </c>
-      <c r="C14" s="315"/>
-      <c r="D14" s="316"/>
-      <c r="E14" s="317"/>
-      <c r="F14" s="331"/>
-      <c r="G14" s="332"/>
-      <c r="H14" s="333"/>
+      <c r="C14" s="324"/>
+      <c r="D14" s="325"/>
+      <c r="E14" s="326"/>
+      <c r="F14" s="321"/>
+      <c r="G14" s="322"/>
+      <c r="H14" s="323"/>
       <c r="I14" s="77"/>
       <c r="J14" s="85"/>
-      <c r="K14" s="352"/>
-      <c r="L14" s="353"/>
-      <c r="M14" s="354"/>
+      <c r="K14" s="330"/>
+      <c r="L14" s="331"/>
+      <c r="M14" s="332"/>
       <c r="N14" s="77"/>
     </row>
     <row r="15" spans="1:14" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -15745,17 +15745,17 @@
       <c r="B15" s="84" t="s">
         <v>215</v>
       </c>
-      <c r="C15" s="315"/>
-      <c r="D15" s="316"/>
-      <c r="E15" s="317"/>
-      <c r="F15" s="331"/>
-      <c r="G15" s="332"/>
-      <c r="H15" s="333"/>
+      <c r="C15" s="324"/>
+      <c r="D15" s="325"/>
+      <c r="E15" s="326"/>
+      <c r="F15" s="321"/>
+      <c r="G15" s="322"/>
+      <c r="H15" s="323"/>
       <c r="I15" s="77"/>
       <c r="J15" s="77"/>
-      <c r="K15" s="352"/>
-      <c r="L15" s="353"/>
-      <c r="M15" s="354"/>
+      <c r="K15" s="330"/>
+      <c r="L15" s="331"/>
+      <c r="M15" s="332"/>
       <c r="N15" s="77"/>
     </row>
     <row r="16" spans="1:14" s="78" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -15763,17 +15763,17 @@
       <c r="B16" s="84" t="s">
         <v>216</v>
       </c>
-      <c r="C16" s="315"/>
-      <c r="D16" s="316"/>
-      <c r="E16" s="317"/>
-      <c r="F16" s="331"/>
-      <c r="G16" s="332"/>
-      <c r="H16" s="333"/>
+      <c r="C16" s="324"/>
+      <c r="D16" s="325"/>
+      <c r="E16" s="326"/>
+      <c r="F16" s="321"/>
+      <c r="G16" s="322"/>
+      <c r="H16" s="323"/>
       <c r="I16" s="77"/>
       <c r="J16" s="77"/>
-      <c r="K16" s="355"/>
-      <c r="L16" s="356"/>
-      <c r="M16" s="357"/>
+      <c r="K16" s="333"/>
+      <c r="L16" s="334"/>
+      <c r="M16" s="335"/>
       <c r="N16" s="77"/>
     </row>
     <row r="17" spans="1:14" s="78" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.3">
@@ -15794,15 +15794,15 @@
     </row>
     <row r="18" spans="1:14" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="77"/>
-      <c r="B18" s="340" t="s">
+      <c r="B18" s="343" t="s">
         <v>217</v>
       </c>
-      <c r="C18" s="343"/>
-      <c r="D18" s="343"/>
-      <c r="E18" s="343"/>
-      <c r="F18" s="343"/>
-      <c r="G18" s="343"/>
-      <c r="H18" s="344"/>
+      <c r="C18" s="344"/>
+      <c r="D18" s="344"/>
+      <c r="E18" s="344"/>
+      <c r="F18" s="344"/>
+      <c r="G18" s="344"/>
+      <c r="H18" s="345"/>
       <c r="I18" s="77"/>
       <c r="J18" s="77"/>
       <c r="K18" s="77"/>
@@ -15813,16 +15813,16 @@
     <row r="19" spans="1:14" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="77"/>
       <c r="B19" s="86"/>
-      <c r="C19" s="334" t="s">
+      <c r="C19" s="315" t="s">
         <v>218</v>
       </c>
-      <c r="D19" s="335"/>
-      <c r="E19" s="335"/>
-      <c r="F19" s="334" t="s">
+      <c r="D19" s="316"/>
+      <c r="E19" s="316"/>
+      <c r="F19" s="315" t="s">
         <v>219</v>
       </c>
-      <c r="G19" s="335"/>
-      <c r="H19" s="336"/>
+      <c r="G19" s="316"/>
+      <c r="H19" s="317"/>
       <c r="I19" s="77"/>
       <c r="J19" s="77"/>
       <c r="K19" s="77"/>
@@ -15835,12 +15835,12 @@
       <c r="B20" s="83" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="315"/>
-      <c r="D20" s="316"/>
-      <c r="E20" s="317"/>
-      <c r="F20" s="331"/>
-      <c r="G20" s="332"/>
-      <c r="H20" s="333"/>
+      <c r="C20" s="324"/>
+      <c r="D20" s="325"/>
+      <c r="E20" s="326"/>
+      <c r="F20" s="321"/>
+      <c r="G20" s="322"/>
+      <c r="H20" s="323"/>
       <c r="I20" s="77"/>
       <c r="J20" s="77"/>
       <c r="K20" s="77"/>
@@ -15853,12 +15853,12 @@
       <c r="B21" s="83" t="s">
         <v>220</v>
       </c>
-      <c r="C21" s="315"/>
-      <c r="D21" s="316"/>
-      <c r="E21" s="317"/>
-      <c r="F21" s="331"/>
-      <c r="G21" s="332"/>
-      <c r="H21" s="333"/>
+      <c r="C21" s="324"/>
+      <c r="D21" s="325"/>
+      <c r="E21" s="326"/>
+      <c r="F21" s="321"/>
+      <c r="G21" s="322"/>
+      <c r="H21" s="323"/>
       <c r="I21" s="77"/>
       <c r="J21" s="77"/>
       <c r="K21" s="77"/>
@@ -15871,12 +15871,12 @@
       <c r="B22" s="83" t="s">
         <v>215</v>
       </c>
-      <c r="C22" s="315"/>
-      <c r="D22" s="316"/>
-      <c r="E22" s="317"/>
-      <c r="F22" s="331"/>
-      <c r="G22" s="332"/>
-      <c r="H22" s="333"/>
+      <c r="C22" s="324"/>
+      <c r="D22" s="325"/>
+      <c r="E22" s="326"/>
+      <c r="F22" s="321"/>
+      <c r="G22" s="322"/>
+      <c r="H22" s="323"/>
       <c r="I22" s="77"/>
       <c r="J22" s="77"/>
       <c r="K22" s="77"/>
@@ -15889,12 +15889,12 @@
       <c r="B23" s="84" t="s">
         <v>216</v>
       </c>
-      <c r="C23" s="315"/>
-      <c r="D23" s="316"/>
-      <c r="E23" s="317"/>
-      <c r="F23" s="331"/>
-      <c r="G23" s="332"/>
-      <c r="H23" s="333"/>
+      <c r="C23" s="324"/>
+      <c r="D23" s="325"/>
+      <c r="E23" s="326"/>
+      <c r="F23" s="321"/>
+      <c r="G23" s="322"/>
+      <c r="H23" s="323"/>
       <c r="I23" s="77"/>
       <c r="J23" s="77"/>
       <c r="K23" s="77"/>
@@ -15905,16 +15905,16 @@
     <row r="24" spans="1:14" s="78" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="77"/>
       <c r="B24" s="87"/>
-      <c r="C24" s="334" t="s">
+      <c r="C24" s="315" t="s">
         <v>221</v>
       </c>
-      <c r="D24" s="335"/>
-      <c r="E24" s="335"/>
-      <c r="F24" s="334" t="s">
+      <c r="D24" s="316"/>
+      <c r="E24" s="316"/>
+      <c r="F24" s="315" t="s">
         <v>222</v>
       </c>
-      <c r="G24" s="335"/>
-      <c r="H24" s="336"/>
+      <c r="G24" s="316"/>
+      <c r="H24" s="317"/>
       <c r="I24" s="77"/>
       <c r="J24" s="77"/>
       <c r="K24" s="77"/>
@@ -15927,12 +15927,12 @@
       <c r="B25" s="83" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="315"/>
-      <c r="D25" s="316"/>
-      <c r="E25" s="317"/>
-      <c r="F25" s="331"/>
-      <c r="G25" s="332"/>
-      <c r="H25" s="333"/>
+      <c r="C25" s="324"/>
+      <c r="D25" s="325"/>
+      <c r="E25" s="326"/>
+      <c r="F25" s="321"/>
+      <c r="G25" s="322"/>
+      <c r="H25" s="323"/>
       <c r="I25" s="77"/>
       <c r="J25" s="77"/>
       <c r="K25" s="88" t="s">
@@ -15947,12 +15947,12 @@
       <c r="B26" s="83" t="s">
         <v>220</v>
       </c>
-      <c r="C26" s="315"/>
-      <c r="D26" s="316"/>
-      <c r="E26" s="317"/>
-      <c r="F26" s="331"/>
-      <c r="G26" s="332"/>
-      <c r="H26" s="333"/>
+      <c r="C26" s="324"/>
+      <c r="D26" s="325"/>
+      <c r="E26" s="326"/>
+      <c r="F26" s="321"/>
+      <c r="G26" s="322"/>
+      <c r="H26" s="323"/>
       <c r="I26" s="77"/>
       <c r="J26" s="77"/>
       <c r="K26" s="90" t="s">
@@ -15967,12 +15967,12 @@
       <c r="B27" s="83" t="s">
         <v>215</v>
       </c>
-      <c r="C27" s="315"/>
-      <c r="D27" s="316"/>
-      <c r="E27" s="317"/>
-      <c r="F27" s="331"/>
-      <c r="G27" s="332"/>
-      <c r="H27" s="333"/>
+      <c r="C27" s="324"/>
+      <c r="D27" s="325"/>
+      <c r="E27" s="326"/>
+      <c r="F27" s="321"/>
+      <c r="G27" s="322"/>
+      <c r="H27" s="323"/>
       <c r="I27" s="77"/>
       <c r="J27" s="77"/>
       <c r="K27" s="90" t="s">
@@ -15987,12 +15987,12 @@
       <c r="B28" s="84" t="s">
         <v>216</v>
       </c>
-      <c r="C28" s="315"/>
-      <c r="D28" s="316"/>
-      <c r="E28" s="317"/>
-      <c r="F28" s="331"/>
-      <c r="G28" s="332"/>
-      <c r="H28" s="333"/>
+      <c r="C28" s="324"/>
+      <c r="D28" s="325"/>
+      <c r="E28" s="326"/>
+      <c r="F28" s="321"/>
+      <c r="G28" s="322"/>
+      <c r="H28" s="323"/>
       <c r="I28" s="77"/>
       <c r="J28" s="77"/>
       <c r="K28" s="92" t="s">
@@ -16007,9 +16007,9 @@
       <c r="B29" s="83" t="s">
         <v>227</v>
       </c>
-      <c r="C29" s="322"/>
-      <c r="D29" s="337"/>
-      <c r="E29" s="338"/>
+      <c r="C29" s="346"/>
+      <c r="D29" s="347"/>
+      <c r="E29" s="348"/>
       <c r="F29" s="69"/>
       <c r="G29" s="95"/>
       <c r="H29" s="95"/>
@@ -16023,16 +16023,16 @@
     <row r="30" spans="1:14" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="77"/>
       <c r="B30" s="87"/>
-      <c r="C30" s="334" t="s">
+      <c r="C30" s="315" t="s">
         <v>228</v>
       </c>
-      <c r="D30" s="335"/>
-      <c r="E30" s="336"/>
-      <c r="F30" s="334" t="s">
+      <c r="D30" s="316"/>
+      <c r="E30" s="317"/>
+      <c r="F30" s="315" t="s">
         <v>288</v>
       </c>
-      <c r="G30" s="335"/>
-      <c r="H30" s="336"/>
+      <c r="G30" s="316"/>
+      <c r="H30" s="317"/>
       <c r="I30" s="77"/>
       <c r="J30" s="77"/>
       <c r="K30" s="96"/>
@@ -16045,14 +16045,14 @@
       <c r="B31" s="83" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="315"/>
-      <c r="D31" s="316"/>
-      <c r="E31" s="317"/>
-      <c r="F31" s="318" t="s">
+      <c r="C31" s="324"/>
+      <c r="D31" s="325"/>
+      <c r="E31" s="326"/>
+      <c r="F31" s="352" t="s">
         <v>299</v>
       </c>
-      <c r="G31" s="319"/>
-      <c r="H31" s="320"/>
+      <c r="G31" s="353"/>
+      <c r="H31" s="354"/>
       <c r="I31" s="97"/>
       <c r="J31" s="97"/>
       <c r="K31" s="74"/>
@@ -16065,14 +16065,14 @@
       <c r="B32" s="83" t="s">
         <v>220</v>
       </c>
-      <c r="C32" s="315"/>
-      <c r="D32" s="316"/>
-      <c r="E32" s="317"/>
-      <c r="F32" s="318" t="s">
+      <c r="C32" s="324"/>
+      <c r="D32" s="325"/>
+      <c r="E32" s="326"/>
+      <c r="F32" s="352" t="s">
         <v>300</v>
       </c>
-      <c r="G32" s="319"/>
-      <c r="H32" s="320"/>
+      <c r="G32" s="353"/>
+      <c r="H32" s="354"/>
       <c r="I32" s="97"/>
       <c r="J32" s="97"/>
       <c r="K32" s="74"/>
@@ -16085,14 +16085,14 @@
       <c r="B33" s="83" t="s">
         <v>215</v>
       </c>
-      <c r="C33" s="315"/>
-      <c r="D33" s="316"/>
-      <c r="E33" s="317"/>
-      <c r="F33" s="318" t="s">
+      <c r="C33" s="324"/>
+      <c r="D33" s="325"/>
+      <c r="E33" s="326"/>
+      <c r="F33" s="352" t="s">
         <v>301</v>
       </c>
-      <c r="G33" s="319"/>
-      <c r="H33" s="320"/>
+      <c r="G33" s="353"/>
+      <c r="H33" s="354"/>
       <c r="I33" s="97"/>
       <c r="J33" s="97"/>
       <c r="K33" s="74"/>
@@ -16105,14 +16105,14 @@
       <c r="B34" s="84" t="s">
         <v>216</v>
       </c>
-      <c r="C34" s="315"/>
-      <c r="D34" s="316"/>
-      <c r="E34" s="317"/>
-      <c r="F34" s="321" t="s">
+      <c r="C34" s="324"/>
+      <c r="D34" s="325"/>
+      <c r="E34" s="326"/>
+      <c r="F34" s="355" t="s">
         <v>302</v>
       </c>
-      <c r="G34" s="319"/>
-      <c r="H34" s="320"/>
+      <c r="G34" s="353"/>
+      <c r="H34" s="354"/>
       <c r="I34" s="97"/>
       <c r="J34" s="97"/>
       <c r="K34" s="74"/>
@@ -16125,9 +16125,9 @@
       <c r="B35" s="84" t="s">
         <v>229</v>
       </c>
-      <c r="C35" s="322"/>
-      <c r="D35" s="323"/>
-      <c r="E35" s="324"/>
+      <c r="C35" s="346"/>
+      <c r="D35" s="356"/>
+      <c r="E35" s="357"/>
       <c r="F35" s="98"/>
       <c r="G35" s="98"/>
       <c r="H35" s="98"/>
@@ -16156,12 +16156,12 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="97"/>
-      <c r="B37" s="325" t="s">
+      <c r="B37" s="358" t="s">
         <v>230</v>
       </c>
-      <c r="C37" s="326"/>
-      <c r="D37" s="326"/>
-      <c r="E37" s="327"/>
+      <c r="C37" s="359"/>
+      <c r="D37" s="359"/>
+      <c r="E37" s="360"/>
       <c r="F37" s="98"/>
       <c r="G37" s="98"/>
       <c r="H37" s="98"/>
@@ -16174,11 +16174,11 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="97"/>
-      <c r="B38" s="328" t="s">
+      <c r="B38" s="361" t="s">
         <v>231</v>
       </c>
-      <c r="C38" s="329"/>
-      <c r="D38" s="330"/>
+      <c r="C38" s="362"/>
+      <c r="D38" s="363"/>
       <c r="E38" s="99"/>
       <c r="F38" s="98"/>
       <c r="G38" s="98"/>
@@ -16192,11 +16192,11 @@
     </row>
     <row r="39" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="97"/>
-      <c r="B39" s="312" t="s">
+      <c r="B39" s="349" t="s">
         <v>232</v>
       </c>
-      <c r="C39" s="313"/>
-      <c r="D39" s="314"/>
+      <c r="C39" s="350"/>
+      <c r="D39" s="351"/>
       <c r="E39" s="100"/>
       <c r="F39" s="98"/>
       <c r="G39" s="98"/>
@@ -16226,6 +16226,54 @@
     </row>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="C19:E19"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="E3:H3"/>
@@ -16242,54 +16290,6 @@
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="E8:H8"/>
     <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B38:D38"/>
   </mergeCells>
   <conditionalFormatting sqref="B4 E4">
     <cfRule type="expression" dxfId="116" priority="7">
@@ -19255,9 +19255,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y116"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G132" sqref="G132"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I36" sqref="H35:I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19860,7 +19860,7 @@
       <c r="F14" s="132"/>
       <c r="G14" s="195"/>
       <c r="H14" s="195" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="I14" s="157" t="s">
         <v>440</v>
@@ -20688,7 +20688,7 @@
       <c r="F38" s="132"/>
       <c r="G38" s="195"/>
       <c r="H38" s="195" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="I38" s="157" t="s">
         <v>440</v>
@@ -22466,7 +22466,7 @@
       </c>
       <c r="F97" s="167"/>
       <c r="G97" s="176" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="H97" s="176"/>
       <c r="I97" s="177" t="s">
@@ -22482,7 +22482,7 @@
       <c r="O97" s="169"/>
       <c r="P97" s="167"/>
       <c r="Q97" s="167" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.3">
@@ -23274,15 +23274,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001185193EED7D7C45B2181268987EEB31" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0398fff93780d69aa75df20e85be37f6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="55e0dd24fae28f1b5dd5f79afbe3cfeb">
     <xsd:element name="properties">
@@ -23396,6 +23387,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -23403,14 +23403,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7243C670-E16E-4DBD-9932-9E3C368D5054}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5245AC5-DF56-430A-AECE-726FB05E2AD0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23422,6 +23414,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7243C670-E16E-4DBD-9932-9E3C368D5054}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>